<commit_message>
Remove testing social media values
</commit_message>
<xml_diff>
--- a/_base/_spreadsheet.xlsx
+++ b/_base/_spreadsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>key</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>google_analytics_id</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
   <si>
     <t>Identifier for Google analytics</t>
@@ -413,11 +410,9 @@
       <c t="s" s="8" r="A3">
         <v>4</v>
       </c>
-      <c t="s" s="7" r="B3">
+      <c s="7" r="B3"/>
+      <c t="s" s="13" r="C3">
         <v>5</v>
-      </c>
-      <c t="s" s="13" r="C3">
-        <v>6</v>
       </c>
       <c s="5" r="D3"/>
       <c s="5" r="E3"/>
@@ -425,13 +420,11 @@
     </row>
     <row r="4">
       <c t="s" s="9" r="A4">
+        <v>6</v>
+      </c>
+      <c s="5" r="B4"/>
+      <c t="s" s="13" r="C4">
         <v>7</v>
-      </c>
-      <c t="s" s="5" r="B4">
-        <v>5</v>
-      </c>
-      <c t="s" s="13" r="C4">
-        <v>8</v>
       </c>
       <c s="5" r="D4"/>
       <c s="5" r="E4"/>
@@ -439,13 +432,11 @@
     </row>
     <row r="5">
       <c t="s" s="9" r="A5">
+        <v>8</v>
+      </c>
+      <c s="5" r="B5"/>
+      <c t="s" s="13" r="C5">
         <v>9</v>
-      </c>
-      <c t="s" s="5" r="B5">
-        <v>5</v>
-      </c>
-      <c t="s" s="13" r="C5">
-        <v>10</v>
       </c>
       <c s="5" r="D5"/>
       <c s="5" r="E5"/>
@@ -453,13 +444,11 @@
     </row>
     <row r="6">
       <c t="s" s="9" r="A6">
+        <v>10</v>
+      </c>
+      <c s="5" r="B6"/>
+      <c t="s" s="13" r="C6">
         <v>11</v>
-      </c>
-      <c t="s" s="5" r="B6">
-        <v>5</v>
-      </c>
-      <c t="s" s="13" r="C6">
-        <v>12</v>
       </c>
       <c s="5" r="D6"/>
       <c s="5" r="E6"/>
@@ -469,7 +458,7 @@
       <c s="9" r="A7"/>
       <c s="5" r="B7"/>
       <c t="s" s="13" r="C7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c s="5" r="D7"/>
       <c s="5" r="E7"/>
@@ -477,13 +466,13 @@
     </row>
     <row r="8">
       <c t="s" s="9" r="A8">
+        <v>13</v>
+      </c>
+      <c t="s" s="5" r="B8">
         <v>14</v>
       </c>
-      <c t="s" s="5" r="B8">
+      <c t="s" s="13" r="C8">
         <v>15</v>
-      </c>
-      <c t="s" s="13" r="C8">
-        <v>16</v>
       </c>
       <c s="5" r="D8"/>
       <c s="5" r="E8"/>
@@ -598,10 +587,10 @@
   <sheetData>
     <row r="1">
       <c t="s" s="11" r="A1">
+        <v>16</v>
+      </c>
+      <c t="s" s="11" r="B1">
         <v>17</v>
-      </c>
-      <c t="s" s="11" r="B1">
-        <v>18</v>
       </c>
       <c s="5" r="C1"/>
       <c s="5" r="D1"/>
@@ -610,10 +599,10 @@
     </row>
     <row r="2">
       <c t="s" s="5" r="A2">
+        <v>18</v>
+      </c>
+      <c t="s" s="3" r="B2">
         <v>19</v>
-      </c>
-      <c t="s" s="3" r="B2">
-        <v>20</v>
       </c>
       <c s="5" r="C2"/>
       <c s="5" r="D2"/>
@@ -622,10 +611,10 @@
     </row>
     <row r="3">
       <c t="s" s="5" r="A3">
+        <v>20</v>
+      </c>
+      <c t="s" s="3" r="B3">
         <v>21</v>
-      </c>
-      <c t="s" s="3" r="B3">
-        <v>22</v>
       </c>
       <c s="5" r="C3"/>
       <c s="5" r="D3"/>
@@ -784,10 +773,10 @@
         <v>0</v>
       </c>
       <c t="s" s="6" r="B1">
+        <v>16</v>
+      </c>
+      <c t="s" s="6" r="C1">
         <v>17</v>
-      </c>
-      <c t="s" s="6" r="C1">
-        <v>18</v>
       </c>
       <c s="5" r="D1"/>
       <c s="5" r="E1"/>
@@ -795,13 +784,13 @@
     </row>
     <row r="2">
       <c t="s" s="7" r="A2">
+        <v>22</v>
+      </c>
+      <c t="s" s="7" r="B2">
         <v>23</v>
       </c>
-      <c t="s" s="7" r="B2">
+      <c t="s" s="12" r="C2">
         <v>24</v>
-      </c>
-      <c t="s" s="12" r="C2">
-        <v>25</v>
       </c>
       <c s="5" r="D2"/>
       <c s="5" r="E2"/>
@@ -809,13 +798,13 @@
     </row>
     <row r="3">
       <c t="s" s="5" r="A3">
+        <v>25</v>
+      </c>
+      <c t="s" s="5" r="B3">
         <v>26</v>
       </c>
-      <c t="s" s="5" r="B3">
+      <c t="s" s="3" r="C3">
         <v>27</v>
-      </c>
-      <c t="s" s="3" r="C3">
-        <v>28</v>
       </c>
       <c s="5" r="D3"/>
       <c s="5" r="E3"/>

</xml_diff>